<commit_message>
rear of rack included
</commit_message>
<xml_diff>
--- a/t03_space_planning/rack_template.xlsx
+++ b/t03_space_planning/rack_template.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peadar/Documents/courses/data_centre_infrastructure/t03_space_planning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grantp\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BAB1CA-D3A8-B14D-9B30-47BFA0699366}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="21460" windowWidth="28040" windowHeight="16200" xr2:uid="{BFCE3DCE-B665-404F-892D-27B95B85C439}"/>
+    <workbookView xWindow="2775" yWindow="21465" windowWidth="28035" windowHeight="16200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,9 +29,23 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>FRONT</t>
+  </si>
+  <si>
+    <t>BACK</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -50,6 +63,13 @@
       <b/>
       <i/>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -75,7 +95,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -95,15 +115,6 @@
       </top>
       <bottom style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="2" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -139,16 +150,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -463,409 +479,470 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F58E7B43-6180-0145-9D59-E638F9A99D7D}">
-  <dimension ref="A2:F45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A3:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
-    <col min="2" max="2" width="7" style="2" customWidth="1"/>
-    <col min="3" max="3" width="57.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="6.5" style="6" customWidth="1"/>
+    <col min="2" max="2" width="3.75" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="3.75" style="2" customWidth="1"/>
+    <col min="5" max="5" width="4.75" style="2" customWidth="1"/>
+    <col min="6" max="6" width="38.5" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
+    <row r="3" spans="1:6" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="C3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
         <v>42</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
-        <f>A3-1</f>
-        <v>41</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
-        <f t="shared" ref="A5:A44" si="0">A4-1</f>
-        <v>40</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
-        <f t="shared" si="0"/>
-        <v>39</v>
+    <row r="6" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <f>A5-1</f>
+        <v>41</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="3"/>
       <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
-        <f t="shared" si="0"/>
-        <v>38</v>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <f t="shared" ref="A7:A46" si="0">A6-1</f>
+        <v>40</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="3"/>
       <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="1"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="1"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
+      <c r="B10" s="1"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="1"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
+      <c r="B11" s="1"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="1"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>35</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
-        <f t="shared" si="0"/>
-        <v>33</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
       <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7">
-        <f t="shared" si="0"/>
-        <v>32</v>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <f t="shared" si="0"/>
+        <v>34</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
       <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7">
-        <f t="shared" si="0"/>
-        <v>31</v>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <f t="shared" si="0"/>
+        <v>33</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
       <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7">
-        <f t="shared" si="0"/>
-        <v>30</v>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
+        <f t="shared" si="0"/>
+        <v>32</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="3"/>
       <c r="D15" s="1"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7">
-        <f t="shared" si="0"/>
-        <v>29</v>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
+        <f t="shared" si="0"/>
+        <v>31</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="3"/>
       <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7">
-        <f t="shared" si="0"/>
-        <v>28</v>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="3"/>
       <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="7">
-        <f t="shared" si="0"/>
-        <v>27</v>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
+        <f t="shared" si="0"/>
+        <v>29</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="3"/>
       <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7">
-        <f t="shared" si="0"/>
-        <v>26</v>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="3"/>
       <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="7">
-        <f t="shared" si="0"/>
-        <v>25</v>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
+        <f t="shared" si="0"/>
+        <v>27</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="3"/>
       <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="7">
-        <f t="shared" si="0"/>
-        <v>24</v>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="6">
+        <f t="shared" si="0"/>
+        <v>26</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="3"/>
       <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="7">
-        <f t="shared" si="0"/>
-        <v>23</v>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="6">
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="3"/>
       <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="7">
-        <f t="shared" si="0"/>
-        <v>22</v>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="6">
+        <f t="shared" si="0"/>
+        <v>24</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="3"/>
       <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="7">
-        <f t="shared" si="0"/>
-        <v>21</v>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="6">
+        <f t="shared" si="0"/>
+        <v>23</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="3"/>
       <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="7">
-        <f t="shared" si="0"/>
-        <v>20</v>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="6">
+        <f t="shared" si="0"/>
+        <v>22</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="3"/>
       <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="7">
-        <f t="shared" si="0"/>
-        <v>19</v>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="6">
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="3"/>
       <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="7">
-        <f t="shared" si="0"/>
-        <v>18</v>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="3"/>
       <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="7">
-        <f t="shared" si="0"/>
-        <v>17</v>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="6">
+        <f t="shared" si="0"/>
+        <v>19</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="3"/>
       <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="7">
-        <f t="shared" si="0"/>
-        <v>16</v>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="6">
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="3"/>
       <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="7">
-        <f t="shared" si="0"/>
-        <v>15</v>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="6">
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="3"/>
       <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="7">
-        <f t="shared" si="0"/>
-        <v>14</v>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="6">
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="3"/>
       <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="7">
-        <f t="shared" si="0"/>
-        <v>13</v>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="6">
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="3"/>
       <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="7">
-        <f t="shared" si="0"/>
-        <v>12</v>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="6">
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="3"/>
       <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="7">
-        <f t="shared" si="0"/>
-        <v>11</v>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="3"/>
       <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="7">
-        <f t="shared" si="0"/>
-        <v>10</v>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="3"/>
       <c r="D35" s="1"/>
-    </row>
-    <row r="36" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="7">
-        <f t="shared" si="0"/>
-        <v>9</v>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="6">
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="3"/>
       <c r="D36" s="1"/>
-    </row>
-    <row r="37" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="7">
-        <f t="shared" si="0"/>
-        <v>8</v>
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="3"/>
       <c r="D37" s="1"/>
-    </row>
-    <row r="38" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="7">
-        <f t="shared" si="0"/>
-        <v>7</v>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="3"/>
       <c r="D38" s="1"/>
-    </row>
-    <row r="39" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="7">
-        <f t="shared" si="0"/>
-        <v>6</v>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="B39" s="1"/>
-      <c r="C39" s="3"/>
+      <c r="C39" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="7">
-        <f t="shared" si="0"/>
-        <v>5</v>
+      <c r="F39" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="6">
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="3"/>
       <c r="D40" s="1"/>
-    </row>
-    <row r="41" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="7">
-        <f t="shared" si="0"/>
-        <v>4</v>
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
       <c r="D41" s="1"/>
-    </row>
-    <row r="42" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="7">
-        <f t="shared" si="0"/>
-        <v>3</v>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
       <c r="D42" s="1"/>
-    </row>
-    <row r="43" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="6">
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
       <c r="D43" s="1"/>
-    </row>
-    <row r="44" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
       <c r="D44" s="1"/>
-    </row>
-    <row r="45" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
+      <c r="C45" s="3"/>
       <c r="D45" s="1"/>
+      <c r="F45" s="3"/>
+    </row>
+    <row r="46" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="1"/>
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="83" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>